<commit_message>
Add test case for log out
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -63,19 +63,34 @@
     <t>User shall be logged in</t>
   </si>
   <si>
-    <t>1-Click on "Logout" link in page Header</t>
-  </si>
-  <si>
-    <t>User shall be log out and redirected to Home Page</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>TAWA_Logout_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify functionality of Logout link for </t>
+    <t>Verify functionality of Logout link for admin</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin shall be logged in</t>
+  </si>
+  <si>
+    <t>1-Click on "Logout" link in page Header in Admin page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Click on "Logout" link in page Header </t>
+  </si>
+  <si>
+    <t>Admin shall be logged out and redirected to Home Page</t>
+  </si>
+  <si>
+    <t>User shall be logged out and redirected to Home Page</t>
+  </si>
+  <si>
+    <t>Crirical</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -467,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,21 +546,36 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update login and signup modules
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Logout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -162,16 +163,7 @@
     <t>Validate login button functionality with invalid user input</t>
   </si>
   <si>
-    <t>User shall be stay at Login page andd error message with"" shall be appeared</t>
-  </si>
-  <si>
     <t>Validate login button functionality with invalid admin input</t>
-  </si>
-  <si>
-    <t>Admin shall be stay at Login page andd error message with"" shall be appeared</t>
-  </si>
-  <si>
-    <t>Check Mandatory Fields</t>
   </si>
   <si>
     <t>1-Open TAWA Website.
@@ -207,9 +199,6 @@
     <t>Nesma Bahgat</t>
   </si>
   <si>
-    <t>An error message shall be appeared with""</t>
-  </si>
-  <si>
     <t>Validate login with valid user name and invalid password</t>
   </si>
   <si>
@@ -228,13 +217,685 @@
 3-Enter invalid user name.
 4-Enter valid password.
 5-Click on "login" button.</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>User shall be stay at Login page andd error message with"The data entered were invalid, please re-enter your data" shall be appeared</t>
+  </si>
+  <si>
+    <t>Admin shall be stay at Login page andd error message with"The data entered were invalid, please re-enter your data" shall be appeared</t>
+  </si>
+  <si>
+    <t>An error message shall be appeared with"The data entered were invalid, please re-enter your data"</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_001</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_002</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_003</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_004</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_005</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_006</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_007</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_008</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_009</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_010</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_011</t>
+  </si>
+  <si>
+    <t>Check Mandatory fields</t>
+  </si>
+  <si>
+    <t>Guest,admin,User</t>
+  </si>
+  <si>
+    <t>Validate login with empty fields</t>
+  </si>
+  <si>
+    <t>Validate "signup" link functionality</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Click on "login" link.</t>
+  </si>
+  <si>
+    <t>User shall be redirected to login page.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter Full name woth length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Check length of full name field</t>
+  </si>
+  <si>
+    <t>Verify Full name field accepts characters</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter full name with characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Verify Full name field accepts characters and spaces</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter full name with characters and spaces only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Verify Full name field accepts characters and spaces only</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "User" radio button.
+4-Leave all fields empty.
+5-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter full name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>An error message should appear with "The data entered were invalid, Please re-enter your data"</t>
+  </si>
+  <si>
+    <t>An error message shall appear with "The data entered were invalid, Please re-enter your data".</t>
+  </si>
+  <si>
+    <t>Check length of User name field</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter User name woth length &gt; 14 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter User name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Verify User name field does not accept spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify uniqueness of User name field </t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter User name already exist.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>An error message should appear with "This username is already reserved. Please enter a different username"</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_012</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_013</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_014</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_015</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_016</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Check length of email field</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter email with length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Validate email field without @ character</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter email without @ char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Validate email field without . character</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter email without . char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter valid email.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Check length of phone field</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number &gt; 20 number.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter valid phone number (numbers only).
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>verify phone field does not accept characters</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>verify phone field does not accept spaces.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and spaces.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>verify phone field does not accept special character.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_018</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_019</t>
+  </si>
+  <si>
+    <t>Verify valid  phone number</t>
+  </si>
+  <si>
+    <t>Verify valid email in email field</t>
+  </si>
+  <si>
+    <t>Verify valid User name which accepts characters, numbers and special character.</t>
+  </si>
+  <si>
+    <t>Verify password less than 8 characters</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enterpassword less than 8 characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>an error message preventing leaving page with "Password must contain number, special characterm upper case, lower case and more than 8 characters.</t>
+  </si>
+  <si>
+    <t>Verify password with characters only</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password with characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Verify password with special characters only</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password with special characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Verify password combination of characters, special character, lower case, upper case and more than 8 characters.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter valid password ,combination of characters, special character, lower case, upper case and more than 8 characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_020</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_021</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_022</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_023</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_024</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_025</t>
+  </si>
+  <si>
+    <t>Verify Password shall be masked</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password.</t>
+  </si>
+  <si>
+    <t>The password shall be masked.</t>
+  </si>
+  <si>
+    <t>Confirm a valid password</t>
+  </si>
+  <si>
+    <t>Verify a confirm password with wrong mismatch</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password that match password field .
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password does not match password field.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_026</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_027</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_028</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_029</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_030</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_031</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_032</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_033</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_034</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_035</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_036</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_037</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_038</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_039</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_040</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_041</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_042</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_043</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_044</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_045</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_046</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_047</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_048</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_049</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_050</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_051</t>
+  </si>
+  <si>
+    <t>The user shall sign up successfully and message appear with " Congratulations! A new account has been created successfully", then user shall redirected to Login page.</t>
+  </si>
+  <si>
+    <t>The user shall sign up successfully and message appear with " Congratulations! A new account has been created successfully", then user shall redirected to login page.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Leave all fields empty.
+5-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter Full name woth length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter full name with characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter full name with characters and spaces only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter full name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter User name woth length &gt; 14 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter User name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter User name already exist.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter email with length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter email without @ char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter email without . char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter valid email.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter valid phone number (numbers only).
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter phone number &gt; 20 number.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter phone number with numbers and characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter phone number with numbers and spaces.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter phone number with numbers and special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enterpassword less than 8 characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter password with characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter password with special characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter valid password ,combination of characters, special character, lower case, upper case and more than 8 characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter password.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter password that match password field .
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-choose "Admin" radio button.
+4-Enter password does not match password field.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_052</t>
+  </si>
+  <si>
+    <t>Verify no chosenn for radio buttons</t>
+  </si>
+  <si>
+    <t>User/Admin</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Leave radio button empty.
+4-Enter valid inputs in all fields.
+5-Click on "SignUp" button.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,8 +918,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +935,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -320,6 +993,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,27 +1310,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-    <col min="3" max="3" width="26" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
-    <col min="6" max="6" width="50.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26" style="5" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="24" style="5" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="23" style="5" customWidth="1"/>
+    <col min="13" max="13" width="19" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,32 +1351,1094 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="90.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +2455,11 @@
     <col min="10" max="10" width="25.28515625" style="5" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,10 +2494,13 @@
         <v>8</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -757,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>32</v>
@@ -766,10 +2520,10 @@
         <v>45</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -783,7 +2537,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>27</v>
@@ -792,10 +2546,10 @@
         <v>28</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -809,7 +2563,7 @@
         <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>44</v>
@@ -818,10 +2572,10 @@
         <v>28</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -832,151 +2586,151 @@
         <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="G6" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -986,10 +2740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,15 +2751,17 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="48.140625" customWidth="1"/>
     <col min="3" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="51.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" customWidth="1"/>
+    <col min="5" max="6" width="51.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28" style="5" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,22 +2778,31 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1053,15 +2818,18 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="4"/>
+      <c r="L2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1077,13 +2845,25 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="L3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test case is updated
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Regestiration" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="AdminPage" sheetId="4" r:id="rId3"/>
-    <sheet name="Logout" sheetId="3" r:id="rId4"/>
+    <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
+    <sheet name="Regestiration" sheetId="1" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId3"/>
+    <sheet name="AdminPage" sheetId="4" r:id="rId4"/>
+    <sheet name="Booking" sheetId="5" r:id="rId5"/>
+    <sheet name="Logout" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="281">
   <si>
     <t>ID</t>
   </si>
@@ -1581,31 +1583,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="26" style="7" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="50.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="50.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.44140625" style="7" customWidth="1"/>
     <col min="10" max="10" width="24" style="5" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="31.88671875" style="5" customWidth="1"/>
     <col min="12" max="12" width="23" style="5" customWidth="1"/>
     <col min="13" max="13" width="19" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="14" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1722,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
@@ -1666,7 +1742,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -1686,7 +1762,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
@@ -1706,7 +1782,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
@@ -1726,7 +1802,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>67</v>
       </c>
@@ -1746,7 +1822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
@@ -1766,7 +1842,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
@@ -1786,7 +1862,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>70</v>
       </c>
@@ -1806,7 +1882,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>71</v>
       </c>
@@ -1826,7 +1902,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="90.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
@@ -1847,7 +1923,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>73</v>
       </c>
@@ -1867,7 +1943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>98</v>
       </c>
@@ -1887,7 +1963,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>99</v>
       </c>
@@ -1907,7 +1983,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>100</v>
       </c>
@@ -1927,7 +2003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>101</v>
       </c>
@@ -1947,7 +2023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>102</v>
       </c>
@@ -1967,7 +2043,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>103</v>
       </c>
@@ -1987,7 +2063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>120</v>
       </c>
@@ -2007,7 +2083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>121</v>
       </c>
@@ -2027,7 +2103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>134</v>
       </c>
@@ -2047,7 +2123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>135</v>
       </c>
@@ -2067,7 +2143,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>136</v>
       </c>
@@ -2087,7 +2163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>137</v>
       </c>
@@ -2107,7 +2183,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>138</v>
       </c>
@@ -2127,7 +2203,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>139</v>
       </c>
@@ -2147,7 +2223,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>147</v>
       </c>
@@ -2167,12 +2243,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>148</v>
       </c>
@@ -2192,7 +2268,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>149</v>
       </c>
@@ -2212,7 +2288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>150</v>
       </c>
@@ -2232,7 +2308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>151</v>
       </c>
@@ -2252,7 +2328,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>152</v>
       </c>
@@ -2272,7 +2348,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>153</v>
       </c>
@@ -2292,7 +2368,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>154</v>
       </c>
@@ -2312,7 +2388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>155</v>
       </c>
@@ -2332,7 +2408,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>156</v>
       </c>
@@ -2353,7 +2429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>157</v>
       </c>
@@ -2373,7 +2449,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
@@ -2393,7 +2469,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>159</v>
       </c>
@@ -2413,7 +2489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>160</v>
       </c>
@@ -2433,7 +2509,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>161</v>
       </c>
@@ -2453,7 +2529,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>162</v>
       </c>
@@ -2473,7 +2549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>163</v>
       </c>
@@ -2493,7 +2569,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>164</v>
       </c>
@@ -2513,7 +2589,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>165</v>
       </c>
@@ -2533,7 +2609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>166</v>
       </c>
@@ -2553,7 +2629,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>167</v>
       </c>
@@ -2573,7 +2649,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>168</v>
       </c>
@@ -2593,7 +2669,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>169</v>
       </c>
@@ -2613,7 +2689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>170</v>
       </c>
@@ -2633,7 +2709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>171</v>
       </c>
@@ -2653,7 +2729,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>172</v>
       </c>
@@ -2673,12 +2749,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>199</v>
       </c>
@@ -2704,33 +2780,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="13" max="13" width="31.109375" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2771,7 +2847,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -2794,7 +2870,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -2820,7 +2896,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -2846,7 +2922,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -2869,7 +2945,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
@@ -2892,7 +2968,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -2912,7 +2988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -2935,7 +3011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -2958,7 +3034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -2981,7 +3057,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
@@ -3009,32 +3085,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" customWidth="1"/>
+    <col min="7" max="7" width="41.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="29" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3072,7 +3146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>206</v>
       </c>
@@ -3101,7 +3175,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>207</v>
       </c>
@@ -3130,7 +3204,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>208</v>
       </c>
@@ -3159,7 +3233,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>209</v>
       </c>
@@ -3191,7 +3265,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>211</v>
       </c>
@@ -3220,7 +3294,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>212</v>
       </c>
@@ -3240,7 +3314,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>213</v>
       </c>
@@ -3263,7 +3337,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>215</v>
       </c>
@@ -3283,8 +3357,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>217</v>
       </c>
@@ -3304,7 +3378,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>219</v>
       </c>
@@ -3324,7 +3398,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>220</v>
       </c>
@@ -3344,7 +3418,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>221</v>
       </c>
@@ -3367,7 +3441,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>223</v>
       </c>
@@ -3390,7 +3464,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>225</v>
       </c>
@@ -3413,8 +3487,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>227</v>
       </c>
@@ -3434,7 +3508,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>228</v>
       </c>
@@ -3457,7 +3531,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>229</v>
       </c>
@@ -3480,7 +3554,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>230</v>
       </c>
@@ -3500,7 +3574,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>231</v>
       </c>
@@ -3526,7 +3600,81 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -3534,22 +3682,22 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
     <col min="3" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" customWidth="1"/>
+    <col min="5" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="33.44140625" customWidth="1"/>
+    <col min="11" max="11" width="39.44140625" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3590,7 +3738,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3617,7 +3765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3644,13 +3792,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case is updated (booking)
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="349">
   <si>
     <t>ID</t>
   </si>
@@ -1138,12 +1138,302 @@
   <si>
     <t>Test Data</t>
   </si>
+  <si>
+    <t>Attachments</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_01</t>
+  </si>
+  <si>
+    <t>Validate the existence of fields</t>
+  </si>
+  <si>
+    <t>User must login with a valid account</t>
+  </si>
+  <si>
+    <t>Valid username: TAWA
+Valid Password: P@$$w0rd
+Valid db card number:
+01234567891012
+valid destination:Turkey
+valid flight number: 2409</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Check the existence of fields</t>
+  </si>
+  <si>
+    <t>Page shall contain fields:
+(See attachements)</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Mahmoud Yasser</t>
+  </si>
+  <si>
+    <t>img: https://ibb.co/ZSWGyKV</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_02</t>
+  </si>
+  <si>
+    <t>Validate the options in "Level of services" list</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Click on "Level of services" dropdown list
+5) Check the list options</t>
+  </si>
+  <si>
+    <t>Dropdown list shall contain 
+‘Egypt Air’, ‘Fly Emirates’ , ‘Qatari Airways’
+ , ‘Turkish Airlines’, ‘Lufthansa’ 
+and ‘Air France’.</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_03</t>
+  </si>
+  <si>
+    <t>Validate the options in "Payment Method" list</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Click on "Payment method" dropdown list
+5) Check the list options</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The ‘payment method’ dropdown list shall contain two methods ‘cash’ and ‘debit card’.</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_04</t>
+  </si>
+  <si>
+    <t>Validate the appearance of "card number" text field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Click on "Payment method" dropdown list and choose debit card
+</t>
+  </si>
+  <si>
+    <t>the ‘card number’ text field shall 
+appear</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_05</t>
+  </si>
+  <si>
+    <t>Validate the restriction on choosing Trip type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Choose One trip type
+5) Try to choose the other type
+</t>
+  </si>
+  <si>
+    <t>User shall be able to choose one
+trip type.</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_06</t>
+  </si>
+  <si>
+    <t>Validate the restriction on choosing Payment method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Choose One payment method
+5) Try to choose the other type
+</t>
+  </si>
+  <si>
+    <t>User shall be able to choose one
+payment method.</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_07</t>
+  </si>
+  <si>
+    <t>Validate the user's ability to click button "book" 
+without filling any field</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Try click on "book" button</t>
+  </si>
+  <si>
+    <t>The "book" button shall not 
+be clickable</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_08</t>
+  </si>
+  <si>
+    <t>Validate the user's ability to click button "book" 
+without completing all data fields</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Fill one field with any data
+5)Try click on "book" button</t>
+  </si>
+  <si>
+    <t>The ‘Book’ button shall be 
+clickable only after filling all data.</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_09</t>
+  </si>
+  <si>
+    <t>Validate restriction on entering data in "NUMBER
+OF SEATS" field</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter letters in "Number of seats" field
+5) complete all other fields
+6) Click on "book" button</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying that it's forbidden to enter any type of data but numbers in "number of seats" field</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_10</t>
+  </si>
+  <si>
+    <t>Validate restriction on entering data in "FLIGHT NUMBER" field</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter letters in "flight number" field
+5) complete all other fields
+6) Click on "book" button</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying that it's forbidden to enter any type of data but numbers in "flight number" field</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_11</t>
+  </si>
+  <si>
+    <t>Validate restriction on entering data in "Debit card number" field</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter letters in "debit card number" field
+5) complete all other fields
+6) Click on "book" button</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying that it's forbidden to enter any type of data but numbers in "debit card number" field</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_12</t>
+  </si>
+  <si>
+    <t>Validate response from the website after booking</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter valid data and complete all fields
+5) Click on "book" button
+6) Check response from website</t>
+  </si>
+  <si>
+    <t>Message shall appear to user:
+See attachments</t>
+  </si>
+  <si>
+    <t>https://ibb.co/BVgnTfK</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_13</t>
+  </si>
+  <si>
+    <t>Validate that user can book one flight</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter valid data and complete all fields
+5) Click on "book" button
+6) Check table Book in TAWA_DB</t>
+  </si>
+  <si>
+    <t>New row shall be added with 
+the data entered</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_14</t>
+  </si>
+  <si>
+    <t>Validate that user can not book more than one flight</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter valid data and complete all fields
+5) Click on "book" button
+6) Repeat steps from 1 to 5</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying
+that user has already booked one
+flight</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_15</t>
+  </si>
+  <si>
+    <t>Validate that user can not book a flight for more than
+4 seats</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) enter "5" IN "number of seats" field
+5) complete all fields and click book</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying
+that user can not book more than 4 seats</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,6 +1459,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1211,7 +1507,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1234,11 +1530,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1281,6 +1592,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1591,7 +1920,7 @@
   </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -3612,73 +3941,593 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="20" t="s">
         <v>59</v>
       </c>
+      <c r="O1" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" ht="122.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="12" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N13" s="21"/>
+      <c r="O13" s="24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N14" s="21"/>
+    </row>
+    <row r="15" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N15" s="21"/>
+    </row>
+    <row r="16" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="N16" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test cases is updated
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -1433,7 +1433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1459,12 +1459,6 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1507,7 +1501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1530,26 +1524,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1604,9 +1583,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3943,27 +3919,28 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" width="18.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4046,11 +4023,11 @@
         <v>290</v>
       </c>
       <c r="N2" s="21"/>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="23" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>292</v>
       </c>
@@ -4084,7 +4061,7 @@
       </c>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:15" ht="122.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>296</v>
       </c>
@@ -4104,7 +4081,7 @@
         <v>298</v>
       </c>
       <c r="G4" s="21"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>299</v>
       </c>
       <c r="I4" s="21"/>
@@ -4423,7 +4400,7 @@
         <v>290</v>
       </c>
       <c r="N13" s="21"/>
-      <c r="O13" s="24" t="s">
+      <c r="O13" s="23" t="s">
         <v>336</v>
       </c>
     </row>

</xml_diff>

<commit_message>
One test case is added
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="353">
   <si>
     <t>ID</t>
   </si>
@@ -1427,6 +1427,27 @@
   <si>
     <t>Error message shall appear saying
 that user can not book more than 4 seats</t>
+  </si>
+  <si>
+    <t>Validate that trip appear in the "Reserved trips" page once
+user books it</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_16</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Now" button
+4) Enter valid data and complete all fields
+5) Click on "book" button
+6) Open Homepage
+7) from navigation bar click on 'Reserved trips" button</t>
+  </si>
+  <si>
+    <t>a trip with the exact same data
+that user entered shall appear 
+in the page</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1586,6 +1607,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3917,16 +3941,16 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.77734375" style="23" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.21875" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="23" customWidth="1"/>
@@ -4505,6 +4529,38 @@
         <v>290</v>
       </c>
       <c r="N16" s="21"/>
+    </row>
+    <row r="17" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21" t="s">
+        <v>290</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test case updated (booking & reserved flights)
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="399">
   <si>
     <t>ID</t>
   </si>
@@ -1103,9 +1103,6 @@
     <t>click on ‘add’ button to submit the form.</t>
   </si>
   <si>
-    <t>Test Data</t>
-  </si>
-  <si>
     <t>Attachments</t>
   </si>
   <si>
@@ -1116,14 +1113,6 @@
   </si>
   <si>
     <t>User must login with a valid account</t>
-  </si>
-  <si>
-    <t>Valid username: TAWA
-Valid Password: P@$$w0rd
-Valid db card number:
-01234567891012
-valid destination:Turkey
-valid flight number: 2409</t>
   </si>
   <si>
     <t>1) Open Homepage
@@ -1394,10 +1383,6 @@
   <si>
     <t>Error message shall appear saying
 that user can not book more than 4 seats</t>
-  </si>
-  <si>
-    <t>Validate that trip appear in the "Reserved trips" page once
-user books it</t>
   </si>
   <si>
     <t>TAWA_BOOKING_16</t>
@@ -1528,6 +1513,120 @@
   </si>
   <si>
     <t>asmaaadmin</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_01</t>
+  </si>
+  <si>
+    <t>Validate that user can go to "Reserved flights" page from home page</t>
+  </si>
+  <si>
+    <t>User must be logged in with
+a valid account and must book
+a flight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open TAWA homepage
+2) From Navigation bar Click on "Reserved
+Flights" button
+</t>
+  </si>
+  <si>
+    <t>Reserved flights page shall load 
+successfully</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_02</t>
+  </si>
+  <si>
+    <t>Validate that reserved flight page has no content if user
+hasn't book any flight yet.</t>
+  </si>
+  <si>
+    <t>User must be logged in with
+a valid account but hasn't book trips</t>
+  </si>
+  <si>
+    <t>1) Open TAWA homepage
+2) From Navigation bar Click on "Reserved
+Flights" button</t>
+  </si>
+  <si>
+    <t>Reserved flights shall has no content</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_03</t>
+  </si>
+  <si>
+    <t>Validate that reserved flight page has information about
+the reserved flight for a user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved flight page shall show :
+Flight Type 
+Airline 
+Service Level 
+Number of seats
+Payment Method 
+</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_04</t>
+  </si>
+  <si>
+    <t>Validate that reserved flights page has a "cancel" button</t>
+  </si>
+  <si>
+    <t>reserved flights page shall
+has a "cancel" button</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_05</t>
+  </si>
+  <si>
+    <t>Validate the functionality of cancel button</t>
+  </si>
+  <si>
+    <t>1) Open TAWA homepage
+2) From Navigation bar Click on "Reserved
+Flights" button
+3) Click on cancel button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flight shall be cancelled and a message
+shall appear saying: Your flight has been Cancelled
+</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_06</t>
+  </si>
+  <si>
+    <t>Validate that there is an option for user to go to homepage after
+the cancellation of a flight</t>
+  </si>
+  <si>
+    <t>A blue button called" Go to Home Page"
+shall appear under the cancellation message</t>
+  </si>
+  <si>
+    <t>TAWA_RESERVED_07</t>
+  </si>
+  <si>
+    <t>Validate the functionality of "go to home page" button</t>
+  </si>
+  <si>
+    <t>1) Open TAWA homepage
+2) From Navigation bar Click on "Reserved
+Flights" button
+3) Click on cancel button
+4) click on "go to home page" button</t>
+  </si>
+  <si>
+    <t>User shall be redirected to homepage successfully</t>
+  </si>
+  <si>
+    <t>Validate that trip appear in the "Reserved flights" page once
+user books it</t>
   </si>
 </sst>
 </file>
@@ -2010,76 +2109,284 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="20" t="s">
         <v>59</v>
       </c>
+      <c r="M1" s="19"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+    </row>
+    <row r="3" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+    </row>
+    <row r="4" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2091,25 +2398,25 @@
       <selection sqref="A1:M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="26" style="7" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="50.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="50.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.44140625" style="7" customWidth="1"/>
     <col min="10" max="10" width="24" style="5" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="31.88671875" style="5" customWidth="1"/>
     <col min="12" max="12" width="23" style="5" customWidth="1"/>
     <col min="13" max="13" width="19" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="14" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2150,7 +2457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
@@ -2170,7 +2477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -2190,7 +2497,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
@@ -2210,7 +2517,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
@@ -2230,7 +2537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>67</v>
       </c>
@@ -2250,7 +2557,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
@@ -2270,7 +2577,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
@@ -2290,7 +2597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>70</v>
       </c>
@@ -2310,7 +2617,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>71</v>
       </c>
@@ -2330,7 +2637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="90.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
@@ -2351,7 +2658,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>73</v>
       </c>
@@ -2371,7 +2678,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>98</v>
       </c>
@@ -2391,7 +2698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>99</v>
       </c>
@@ -2411,7 +2718,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>100</v>
       </c>
@@ -2431,7 +2738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>101</v>
       </c>
@@ -2451,7 +2758,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>102</v>
       </c>
@@ -2471,7 +2778,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>103</v>
       </c>
@@ -2491,7 +2798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>120</v>
       </c>
@@ -2511,7 +2818,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>121</v>
       </c>
@@ -2531,7 +2838,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>134</v>
       </c>
@@ -2551,7 +2858,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>135</v>
       </c>
@@ -2571,7 +2878,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>136</v>
       </c>
@@ -2591,7 +2898,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>137</v>
       </c>
@@ -2611,7 +2918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>138</v>
       </c>
@@ -2631,7 +2938,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>139</v>
       </c>
@@ -2651,7 +2958,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>147</v>
       </c>
@@ -2671,12 +2978,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>148</v>
       </c>
@@ -2696,7 +3003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>149</v>
       </c>
@@ -2716,7 +3023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>150</v>
       </c>
@@ -2736,7 +3043,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>151</v>
       </c>
@@ -2756,7 +3063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>152</v>
       </c>
@@ -2776,7 +3083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>153</v>
       </c>
@@ -2796,7 +3103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>154</v>
       </c>
@@ -2816,7 +3123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>155</v>
       </c>
@@ -2836,7 +3143,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="90.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>156</v>
       </c>
@@ -2857,7 +3164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>157</v>
       </c>
@@ -2877,7 +3184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
@@ -2897,7 +3204,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>159</v>
       </c>
@@ -2917,7 +3224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>160</v>
       </c>
@@ -2937,7 +3244,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>161</v>
       </c>
@@ -2957,7 +3264,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>162</v>
       </c>
@@ -2977,7 +3284,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>163</v>
       </c>
@@ -2997,7 +3304,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>164</v>
       </c>
@@ -3017,7 +3324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>165</v>
       </c>
@@ -3037,7 +3344,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>166</v>
       </c>
@@ -3057,7 +3364,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>167</v>
       </c>
@@ -3077,7 +3384,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>168</v>
       </c>
@@ -3097,7 +3404,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>169</v>
       </c>
@@ -3117,7 +3424,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>170</v>
       </c>
@@ -3137,7 +3444,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>171</v>
       </c>
@@ -3157,7 +3464,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>172</v>
       </c>
@@ -3177,12 +3484,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>199</v>
       </c>
@@ -3216,25 +3523,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="13" max="13" width="31.109375" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3275,7 +3582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -3298,7 +3605,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -3324,7 +3631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -3350,7 +3657,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -3373,7 +3680,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
@@ -3396,7 +3703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -3416,7 +3723,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -3439,7 +3746,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -3462,7 +3769,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -3485,7 +3792,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
@@ -3517,28 +3824,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" customWidth="1"/>
+    <col min="7" max="7" width="41.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="29" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3883,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>206</v>
       </c>
@@ -3587,7 +3894,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>250</v>
@@ -3605,7 +3912,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>207</v>
       </c>
@@ -3616,7 +3923,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>251</v>
@@ -3634,7 +3941,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>208</v>
       </c>
@@ -3645,7 +3952,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>264</v>
@@ -3663,7 +3970,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>209</v>
       </c>
@@ -3674,7 +3981,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>265</v>
@@ -3695,7 +4002,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>211</v>
       </c>
@@ -3706,7 +4013,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>267</v>
@@ -3724,7 +4031,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>212</v>
       </c>
@@ -3735,16 +4042,16 @@
         <v>16</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>254</v>
@@ -3756,7 +4063,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>213</v>
       </c>
@@ -3767,16 +4074,16 @@
         <v>16</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>255</v>
@@ -3785,10 +4092,10 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>237</v>
@@ -3797,16 +4104,16 @@
         <v>16</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>255</v>
@@ -3815,7 +4122,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>214</v>
       </c>
@@ -3826,16 +4133,16 @@
         <v>16</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>253</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>255</v>
@@ -3844,7 +4151,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>215</v>
       </c>
@@ -3855,16 +4162,16 @@
         <v>16</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>216</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>254</v>
@@ -3876,7 +4183,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>217</v>
       </c>
@@ -3887,16 +4194,16 @@
         <v>16</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>218</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>254</v>
@@ -3908,7 +4215,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>219</v>
       </c>
@@ -3919,16 +4226,16 @@
         <v>16</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>220</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>254</v>
@@ -3940,8 +4247,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:13" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>221</v>
       </c>
@@ -3952,16 +4259,16 @@
         <v>16</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>226</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>255</v>
@@ -3970,7 +4277,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>222</v>
       </c>
@@ -3981,16 +4288,16 @@
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>227</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>254</v>
@@ -4002,7 +4309,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>223</v>
       </c>
@@ -4013,16 +4320,16 @@
         <v>16</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>228</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>254</v>
@@ -4034,7 +4341,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>224</v>
       </c>
@@ -4045,16 +4352,16 @@
         <v>16</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>229</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>255</v>
@@ -4063,7 +4370,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>225</v>
       </c>
@@ -4074,16 +4381,16 @@
         <v>16</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>230</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>255</v>
@@ -4106,42 +4413,42 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>364</v>
-      </c>
-      <c r="B1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>366</v>
-      </c>
-      <c r="B4" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>367</v>
       </c>
       <c r="B5" s="25">
         <v>1234</v>
@@ -4163,31 +4470,28 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="23" customWidth="1"/>
+    <col min="7" max="8" width="27" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="23"/>
+    <col min="10" max="10" width="9.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="25" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4201,586 +4505,552 @@
         <v>10</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="B2" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21" t="s">
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="C3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F3" s="22" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="O3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="C4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F4" s="22" t="s">
+      <c r="H4" s="21"/>
+      <c r="I4" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="O4" s="22"/>
+    </row>
+    <row r="5" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N4" s="21"/>
-    </row>
-    <row r="5" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="C5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="H5" s="21"/>
+      <c r="I5" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="O5" s="22"/>
+    </row>
+    <row r="6" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N5" s="21"/>
-    </row>
-    <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="C6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="F6" s="21"/>
+      <c r="G6" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N6" s="21"/>
-    </row>
-    <row r="7" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="C7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F7" s="22" t="s">
+      <c r="H7" s="21"/>
+      <c r="I7" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="O7" s="22"/>
+    </row>
+    <row r="8" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22" t="s">
+      <c r="B8" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N7" s="21"/>
-    </row>
-    <row r="8" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="C8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F8" s="22" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="O8" s="22"/>
+    </row>
+    <row r="9" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22" t="s">
+      <c r="B9" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="F9" s="21"/>
+      <c r="G9" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F9" s="22" t="s">
+      <c r="H9" s="21"/>
+      <c r="I9" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M9" s="21"/>
+      <c r="O9" s="22"/>
+    </row>
+    <row r="10" spans="1:15" ht="144" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22" t="s">
+      <c r="B10" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="C10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="H10" s="21"/>
+      <c r="I10" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M10" s="21"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22" t="s">
+      <c r="B11" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="C11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F11" s="22" t="s">
+      <c r="H11" s="21"/>
+      <c r="I11" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M11" s="21"/>
+      <c r="O11" s="22"/>
+    </row>
+    <row r="12" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22" t="s">
+      <c r="B12" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N11" s="21"/>
-    </row>
-    <row r="12" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="C12" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F12" s="22" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M12" s="21"/>
+      <c r="O12" s="22"/>
+    </row>
+    <row r="13" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N12" s="21"/>
-    </row>
-    <row r="13" spans="1:15" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="C13" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M13" s="21"/>
+      <c r="N13" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22" t="s">
+      <c r="O13" s="22"/>
+    </row>
+    <row r="14" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="C14" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="F14" s="21"/>
+      <c r="G14" s="22" t="s">
         <v>327</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F14" s="22" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M14" s="21"/>
+      <c r="O14" s="22"/>
+    </row>
+    <row r="15" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N14" s="21"/>
-    </row>
-    <row r="15" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="C15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M15" s="21"/>
+      <c r="O15" s="22"/>
+    </row>
+    <row r="16" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22" t="s">
+      <c r="B16" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N15" s="21"/>
-    </row>
-    <row r="16" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="C16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F16" s="22" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="O16" s="22"/>
+    </row>
+    <row r="17" spans="1:15" ht="144" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22" t="s">
+      <c r="B17" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>337</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="N16" s="21"/>
-    </row>
-    <row r="17" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="G17" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21" t="s">
-        <v>278</v>
-      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="J17" s="21"/>
       <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21" t="s">
-        <v>279</v>
-      </c>
+      <c r="L17" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="O17" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4795,22 +5065,22 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
     <col min="3" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" customWidth="1"/>
+    <col min="5" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="33.44140625" customWidth="1"/>
+    <col min="11" max="11" width="39.44140625" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4851,7 +5121,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4878,7 +5148,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4905,13 +5175,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add home page and destination test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
-    <sheet name="Registeration" sheetId="1" r:id="rId2"/>
-    <sheet name="Login" sheetId="2" r:id="rId3"/>
-    <sheet name="AdminPage" sheetId="4" r:id="rId4"/>
-    <sheet name="Test-Data" sheetId="7" r:id="rId5"/>
-    <sheet name="Booking" sheetId="5" r:id="rId6"/>
-    <sheet name="Logout" sheetId="3" r:id="rId7"/>
+    <sheet name="Home Page" sheetId="8" r:id="rId2"/>
+    <sheet name="Destination" sheetId="9" r:id="rId3"/>
+    <sheet name="Registeration" sheetId="1" r:id="rId4"/>
+    <sheet name="Login" sheetId="2" r:id="rId5"/>
+    <sheet name="AdminPage" sheetId="4" r:id="rId6"/>
+    <sheet name="Test-Data" sheetId="7" r:id="rId7"/>
+    <sheet name="Booking" sheetId="5" r:id="rId8"/>
+    <sheet name="Logout" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="548">
   <si>
     <t>ID</t>
   </si>
@@ -1726,12 +1728,508 @@
   <si>
     <t>User shall be redirected to homepage successfully</t>
   </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that the user after login will be able to view home page  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-go to the website url
+2-login with the mentioned account in the test data 
+3-validate that the user will be redirected to the home page </t>
+  </si>
+  <si>
+    <t>Valid user name:tawa
+Valid Password:P@$$w0rd</t>
+  </si>
+  <si>
+    <t>the user will be redirected to the
+ home page and will be able to
+ see the destinations and the top rated destination</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Maysoon</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that the gues (unregistered )will be able to view home page  </t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-go to the website url
+2-validate that the guest will be redirected to the home page </t>
+  </si>
+  <si>
+    <t>the guest will be redirected to the
+ home page and will be able to
+ see the destinations and the top rated destination</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_001</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validate that The homepage contains a ‘sign up’ button in the navigation bar.</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check that the navigation bar has sign up button</t>
+  </si>
+  <si>
+    <t>the home page shall contain sign up button 
+in the navigation bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low </t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>the navigation bar is contained
+ signup link not button</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_002</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_004</t>
+  </si>
+  <si>
+    <t>Validate that the guest will be redircted to the sign up form when click on 
+the signup button in the navigation bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-go to the website url
+2-the home page will open 
+3- check that the navigation bar has sign up button
+4-click on sign up </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user shall be redirected to the sign up form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user has been redirected
+ to the sign up form </t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_005</t>
+  </si>
+  <si>
+    <t>Validate what will happen when autherized user click on 
+the signup button in the navigation bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logined user </t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_038</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validate that The homepage contains a ‘login’ button in the navigation bar.</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check that the navigation bar has login button</t>
+  </si>
+  <si>
+    <t>the home page shall contain login button 
+in the navigation bar</t>
+  </si>
+  <si>
+    <t>the navigation bar is contained
+ login link not button</t>
+  </si>
+  <si>
+    <r>
+      <t>TAWA_SRS_FR_0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>95</t>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_HomePage_007</t>
+  </si>
+  <si>
+    <t>validate that the home page  contains a photo gallery of the top travel destinations.</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check the  a photo gallery of the top travel destinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the home page shall  contain a photo gallery of
+ the top travel destinations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the home page doesn't contain
+ the photo gallery </t>
+  </si>
+  <si>
+    <r>
+      <t>TAWA_SRS_FR_096</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_HomePage_008</t>
+  </si>
+  <si>
+    <t>validate that  The home page contains ‘Grid view’ button.</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check the The home page contains ‘Grid view’ button.</t>
+  </si>
+  <si>
+    <t>the home page shall  contain a grid view button</t>
+  </si>
+  <si>
+    <t>the grid view button is exsist</t>
+  </si>
+  <si>
+    <r>
+      <t>TAWA_SRS_FR_097</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_HomePage_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that the grid view button in the home page is clickable and 
+ the distenations are affected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+the page in the list view </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on the grid view button</t>
+  </si>
+  <si>
+    <t>the displayed details will be changed from the
+ list view to the grid view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the diestinations are displayed in 
+grid view instead of list view </t>
+  </si>
+  <si>
+    <r>
+      <t>TAWA_SRS_FR_098</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_HomePage_010</t>
+  </si>
+  <si>
+    <t>validate that  The home page contains ‘list view’ button.</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check the The home page contains ‘list view’ button.</t>
+  </si>
+  <si>
+    <t>the home page shall  contain a list view button</t>
+  </si>
+  <si>
+    <t>the list view button is exsist</t>
+  </si>
+  <si>
+    <r>
+      <t>TAWA_SRS_FR_099</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_HomePage_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that the list view button in the home page is clickable and 
+ the distenations are affected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+the page in the grid view </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on the list view button</t>
+  </si>
+  <si>
+    <t>the displayed details will be changed from the
+ list view to the list view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the diestinations are displayed in 
+list view instead of list view </t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that when click on the destination read more button the user 
+will redirected to the destination details page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user shall be redirected to the destination 
+details page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user  redirected to the destination details page </t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_107
+TAWA_SRS_FR_108</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_013</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_109</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that destination details contains a list of avalibale places </t>
+  </si>
+  <si>
+    <t>User / Guest</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check the avaibale places in this country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will find a list 
+of available places </t>
+  </si>
+  <si>
+    <t>a list of available places are exsist in the page</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_110</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that destination details contains a list of the best restaurants  </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check the list of the best restaurants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will find a list 
+of the best restaurants </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no list of best restaurant </t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_111</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_003</t>
+  </si>
+  <si>
+    <t>validate that destination details contains a list of the available airlines</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>logged in user</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check the list of the available airlines</t>
+  </si>
+  <si>
+    <t>there is no list of  available airlines</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_112
+TAWA_SRS_FR_117 
+TAWA_SRS_FR_118</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_004</t>
+  </si>
+  <si>
+    <t>validate that The travel destination details shall be contains  the ‘rating &amp; feedback’ 
+of this destination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- click in write feedback button </t>
+  </si>
+  <si>
+    <t>the user will be able redircted in the page that avle him to rate the destination and write his feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user is redirected </t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_113</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_005</t>
+  </si>
+  <si>
+    <t>validate that the page has book button</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check if the book button is exsist</t>
+  </si>
+  <si>
+    <t>the page contains book button</t>
+  </si>
+  <si>
+    <t>the button is exsist</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_114
+TAWA_SRS_FR_115</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_006</t>
+  </si>
+  <si>
+    <t>validate that the user will redirected to the booking 
+page when click on book button</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- click on the book button is exsist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will redirected to the booking page </t>
+  </si>
+  <si>
+    <t>TAWA_Destination_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that the unsigned user will not be 
+able to see the book or feedback buttons </t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check book button
+6- check feedback button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no buttons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttons are exsisted </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1768,8 +2266,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1806,8 +2316,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1830,12 +2346,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1899,6 +2430,71 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2209,7 +2805,7 @@
   </sheetPr>
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2488,6 +3084,845 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="8" max="8" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>434</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N2" s="27"/>
+    </row>
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="27" t="s">
+        <v>437</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="F3" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>443</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>444</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>451</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>458</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>432</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N6" s="40"/>
+    </row>
+    <row r="7" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>459</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>474</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>479</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>480</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>481</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="30" t="s">
+        <v>484</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>486</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="29" t="s">
+        <v>488</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>492</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>494</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>496</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K12" s="28"/>
+      <c r="L12" s="30" t="s">
+        <v>497</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="27" t="s">
+        <v>498</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="29" t="s">
+        <v>500</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="42" t="s">
+        <v>503</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="29" t="s">
+        <v>500</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="N14" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="43" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>507</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="29" t="s">
+        <v>509</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
+        <v>510</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43" t="s">
+        <v>435</v>
+      </c>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43" t="s">
+        <v>511</v>
+      </c>
+      <c r="M2" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="N2" s="43"/>
+    </row>
+    <row r="3" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="42" t="s">
+        <v>512</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>514</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>508</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="29" t="s">
+        <v>515</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="J3" t="s">
+        <v>449</v>
+      </c>
+      <c r="L3" t="s">
+        <v>517</v>
+      </c>
+      <c r="M3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>520</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>523</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>510</v>
+      </c>
+      <c r="J4" t="s">
+        <v>449</v>
+      </c>
+      <c r="L4" t="s">
+        <v>524</v>
+      </c>
+      <c r="M4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
+        <v>525</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>526</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>527</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>528</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>529</v>
+      </c>
+      <c r="J5" t="s">
+        <v>435</v>
+      </c>
+      <c r="L5" t="s">
+        <v>530</v>
+      </c>
+      <c r="M5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
+        <v>531</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>532</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>533</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>534</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>535</v>
+      </c>
+      <c r="J6" t="s">
+        <v>435</v>
+      </c>
+      <c r="L6" t="s">
+        <v>536</v>
+      </c>
+      <c r="M6" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="42" t="s">
+        <v>537</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>539</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>540</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>541</v>
+      </c>
+      <c r="J7" t="s">
+        <v>435</v>
+      </c>
+      <c r="L7" t="s">
+        <v>530</v>
+      </c>
+      <c r="M7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="47"/>
+      <c r="B8" s="48" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>543</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="E8" s="48"/>
+      <c r="F8" s="39" t="s">
+        <v>545</v>
+      </c>
+      <c r="G8" s="47"/>
+      <c r="H8" s="49" t="s">
+        <v>546</v>
+      </c>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47" t="s">
+        <v>449</v>
+      </c>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47" t="s">
+        <v>547</v>
+      </c>
+      <c r="M8" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="N8" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
@@ -3612,7 +5047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -3917,7 +5352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
@@ -4585,7 +6020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -4643,7 +6078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5"/>
@@ -5288,7 +6723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Tc updated after retest
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Booking" sheetId="5" r:id="rId9"/>
     <sheet name="Logout" sheetId="3" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="649">
   <si>
     <t>ID</t>
   </si>
@@ -2287,9 +2287,6 @@
     <t>TAWA_BOOKING_BUG_01</t>
   </si>
   <si>
-    <t>card number field exists anyway</t>
-  </si>
-  <si>
     <t>user can not choose more than one type</t>
   </si>
   <si>
@@ -2313,9 +2310,6 @@
     <t>TAWA_BOOKING_BUG_02</t>
   </si>
   <si>
-    <t>field accept negative</t>
-  </si>
-  <si>
     <t>message appeared</t>
   </si>
   <si>
@@ -2547,12 +2541,24 @@
   <si>
     <t>User redirected to homepage successfully</t>
   </si>
+  <si>
+    <t>Solved</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> card number field exists anyway
+Update: card number only appears when 
+user chooses debit card option</t>
+  </si>
+  <si>
+    <t>field accept negative
+UPDATE: field doesn't accept negative</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2609,8 +2615,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2661,6 +2674,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -2716,13 +2734,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2886,11 +2905,21 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3198,7 +3227,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -3260,29 +3289,29 @@
     </row>
     <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C2" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="58" t="s">
+        <v>613</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>614</v>
+      </c>
+      <c r="F2" s="58" t="s">
         <v>615</v>
       </c>
-      <c r="E2" s="58" t="s">
-        <v>616</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>617</v>
-      </c>
       <c r="G2" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H2" s="57"/>
       <c r="I2" s="57" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="J2" s="57" t="s">
         <v>244</v>
@@ -3292,29 +3321,29 @@
     </row>
     <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C3" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="58" t="s">
+        <v>619</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>620</v>
+      </c>
+      <c r="F3" s="57" t="s">
         <v>621</v>
       </c>
-      <c r="E3" s="58" t="s">
-        <v>622</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>623</v>
-      </c>
       <c r="G3" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H3" s="57"/>
       <c r="I3" s="57" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="J3" s="57" t="s">
         <v>244</v>
@@ -3324,63 +3353,63 @@
     </row>
     <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C4" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H4" s="57"/>
       <c r="I4" s="57" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J4" s="57" t="s">
         <v>244</v>
       </c>
       <c r="K4" s="57"/>
       <c r="L4" s="57" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J5" s="57" t="s">
         <v>244</v>
@@ -3390,29 +3419,29 @@
     </row>
     <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C6" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F6" s="58" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H6" s="57"/>
       <c r="I6" s="58" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J6" s="57" t="s">
         <v>244</v>
@@ -3422,29 +3451,29 @@
     </row>
     <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C7" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F7" s="58" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G7" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="58" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J7" s="57" t="s">
         <v>244</v>
@@ -3454,29 +3483,29 @@
     </row>
     <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="57" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="F8" s="57" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="57" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J8" s="57" t="s">
         <v>244</v>
@@ -4515,29 +4544,29 @@
     </row>
     <row r="2" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C2" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="58" t="s">
+        <v>590</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>591</v>
+      </c>
+      <c r="F2" s="58" t="s">
         <v>592</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="G2" s="57" t="s">
         <v>593</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>594</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>595</v>
       </c>
       <c r="H2" s="57"/>
       <c r="I2" s="57" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J2" s="57" t="s">
         <v>244</v>
@@ -4546,31 +4575,31 @@
     </row>
     <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="59" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C3" s="59" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E3" s="60" t="s">
+        <v>597</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>598</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>599</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>600</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>601</v>
       </c>
       <c r="H3" s="55" t="s">
         <v>575</v>
       </c>
       <c r="I3" s="59" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J3" s="59" t="s">
         <v>244</v>
@@ -4579,29 +4608,29 @@
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C4" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H4" s="57"/>
       <c r="I4" s="57" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J4" s="57" t="s">
         <v>244</v>
@@ -4610,29 +4639,29 @@
     </row>
     <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J5" s="57" t="s">
         <v>244</v>
@@ -7387,8 +7416,8 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7579,38 +7608,38 @@
       <c r="L5" s="51"/>
     </row>
     <row r="6" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="61" t="s">
         <v>253</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="62" t="s">
         <v>551</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="G6" s="53" t="s">
-        <v>371</v>
-      </c>
-      <c r="H6" s="55" t="s">
+      <c r="G6" s="61" t="s">
+        <v>646</v>
+      </c>
+      <c r="H6" s="63" t="s">
         <v>575</v>
       </c>
-      <c r="I6" s="54" t="s">
-        <v>576</v>
-      </c>
-      <c r="J6" s="53" t="s">
+      <c r="I6" s="62" t="s">
+        <v>647</v>
+      </c>
+      <c r="J6" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -7636,7 +7665,7 @@
       </c>
       <c r="H7" s="51"/>
       <c r="I7" s="51" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J7" s="51" t="s">
         <v>244</v>
@@ -7668,7 +7697,7 @@
       </c>
       <c r="H8" s="51"/>
       <c r="I8" s="51" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J8" s="51" t="s">
         <v>244</v>
@@ -7700,7 +7729,7 @@
       </c>
       <c r="H9" s="51"/>
       <c r="I9" s="51" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J9" s="51" t="s">
         <v>244</v>
@@ -7732,7 +7761,7 @@
       </c>
       <c r="H10" s="51"/>
       <c r="I10" s="51" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J10" s="51" t="s">
         <v>244</v>
@@ -7757,14 +7786,14 @@
         <v>556</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G11" s="51" t="s">
         <v>229</v>
       </c>
       <c r="H11" s="51"/>
       <c r="I11" s="51" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J11" s="51" t="s">
         <v>244</v>
@@ -7796,7 +7825,7 @@
       </c>
       <c r="H12" s="51"/>
       <c r="I12" s="51" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J12" s="51" t="s">
         <v>244</v>
@@ -7805,38 +7834,38 @@
       <c r="L12" s="51"/>
     </row>
     <row r="13" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="62" t="s">
         <v>573</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="62" t="s">
+        <v>580</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>559</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>646</v>
+      </c>
+      <c r="H13" s="63" t="s">
         <v>581</v>
       </c>
-      <c r="F13" s="54" t="s">
-        <v>559</v>
-      </c>
-      <c r="G13" s="53" t="s">
-        <v>371</v>
-      </c>
-      <c r="H13" s="55" t="s">
-        <v>582</v>
-      </c>
-      <c r="I13" s="53" t="s">
-        <v>583</v>
-      </c>
-      <c r="J13" s="53" t="s">
+      <c r="I13" s="62" t="s">
+        <v>648</v>
+      </c>
+      <c r="J13" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
     </row>
     <row r="14" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
@@ -7862,7 +7891,7 @@
       </c>
       <c r="H14" s="51"/>
       <c r="I14" s="51" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J14" s="51" t="s">
         <v>244</v>
@@ -7896,7 +7925,7 @@
       </c>
       <c r="H15" s="51"/>
       <c r="I15" s="51" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J15" s="51" t="s">
         <v>244</v>
@@ -7927,10 +7956,10 @@
         <v>371</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>244</v>
@@ -7962,7 +7991,7 @@
       </c>
       <c r="H17" s="51"/>
       <c r="I17" s="51" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J17" s="51" t="s">
         <v>244</v>
@@ -7994,7 +8023,7 @@
       </c>
       <c r="H18" s="51"/>
       <c r="I18" s="51" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J18" s="51" t="s">
         <v>244</v>

</xml_diff>

<commit_message>
Home, reserved, header Test cases reviewed by Maysoon Magdy
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="652">
   <si>
     <t>ID</t>
   </si>
@@ -2552,6 +2552,15 @@
   <si>
     <t>field accept negative
 UPDATE: field doesn't accept negative</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maysoon Magdy </t>
+  </si>
+  <si>
+    <t>Maysoon Magdy</t>
   </si>
 </sst>
 </file>
@@ -3227,8 +3236,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3316,7 +3325,9 @@
       <c r="J2" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="57"/>
+      <c r="K2" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L2" s="57"/>
     </row>
     <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -3348,7 +3359,9 @@
       <c r="J3" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="57"/>
+      <c r="K3" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -3380,7 +3393,9 @@
       <c r="J4" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="57"/>
+      <c r="K4" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L4" s="57" t="s">
         <v>627</v>
       </c>
@@ -3414,7 +3429,9 @@
       <c r="J5" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="57"/>
+      <c r="K5" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L5" s="57"/>
     </row>
     <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -3446,7 +3463,9 @@
       <c r="J6" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K6" s="57"/>
+      <c r="K6" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -3478,7 +3497,9 @@
       <c r="J7" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="57"/>
+      <c r="K7" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -3510,7 +3531,9 @@
       <c r="J8" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="57"/>
+      <c r="K8" s="57" t="s">
+        <v>651</v>
+      </c>
       <c r="L8" s="57"/>
     </row>
   </sheetData>
@@ -7416,8 +7439,8 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7432,8 +7455,7 @@
     <col min="8" max="8" width="22.88671875" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.44140625" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="59.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="59.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="15"/>
   </cols>
@@ -7470,12 +7492,14 @@
         <v>49</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="M1" s="56"/>
+      <c r="M1" s="56" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51" t="s">
@@ -7506,10 +7530,13 @@
       <c r="J2" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="51"/>
+      <c r="K2" s="51" t="s">
+        <v>547</v>
+      </c>
       <c r="L2" s="51" t="s">
-        <v>547</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
@@ -7541,7 +7568,10 @@
         <v>244</v>
       </c>
       <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="L3" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M3" s="51"/>
     </row>
     <row r="4" spans="1:13" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="51" t="s">
@@ -7573,7 +7603,10 @@
         <v>244</v>
       </c>
       <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="L4" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M4" s="51"/>
     </row>
     <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="51" t="s">
@@ -7605,7 +7638,10 @@
         <v>244</v>
       </c>
       <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
+      <c r="L5" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
@@ -7639,7 +7675,10 @@
         <v>244</v>
       </c>
       <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
+      <c r="L6" s="61" t="s">
+        <v>650</v>
+      </c>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -7671,7 +7710,10 @@
         <v>244</v>
       </c>
       <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
+      <c r="L7" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="51" t="s">
@@ -7703,7 +7745,10 @@
         <v>244</v>
       </c>
       <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
+      <c r="L8" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M8" s="51"/>
     </row>
     <row r="9" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
@@ -7735,7 +7780,10 @@
         <v>244</v>
       </c>
       <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
+      <c r="L9" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
@@ -7767,7 +7815,10 @@
         <v>244</v>
       </c>
       <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
+      <c r="L10" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M10" s="51"/>
     </row>
     <row r="11" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="51" t="s">
@@ -7799,7 +7850,10 @@
         <v>244</v>
       </c>
       <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
+      <c r="L11" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M11" s="51"/>
     </row>
     <row r="12" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="51" t="s">
@@ -7831,7 +7885,10 @@
         <v>244</v>
       </c>
       <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
+      <c r="L12" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M12" s="51"/>
     </row>
     <row r="13" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="61" t="s">
@@ -7865,7 +7922,10 @@
         <v>244</v>
       </c>
       <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
+      <c r="L13" s="61" t="s">
+        <v>650</v>
+      </c>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
@@ -7896,10 +7956,13 @@
       <c r="J14" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="K14" s="51"/>
+      <c r="K14" s="51" t="s">
+        <v>273</v>
+      </c>
       <c r="L14" s="51" t="s">
-        <v>273</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="M14" s="51"/>
     </row>
     <row r="15" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A15" s="51" t="s">
@@ -7931,7 +7994,10 @@
         <v>244</v>
       </c>
       <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
+      <c r="L15" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M15" s="51"/>
     </row>
     <row r="16" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
@@ -7965,9 +8031,12 @@
         <v>244</v>
       </c>
       <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-    </row>
-    <row r="17" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="L16" s="53" t="s">
+        <v>650</v>
+      </c>
+      <c r="M16" s="53"/>
+    </row>
+    <row r="17" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="51" t="s">
         <v>282</v>
       </c>
@@ -7997,9 +8066,12 @@
         <v>244</v>
       </c>
       <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-    </row>
-    <row r="18" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="L17" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M17" s="51"/>
+    </row>
+    <row r="18" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
         <v>346</v>
       </c>
@@ -8029,9 +8101,12 @@
         <v>244</v>
       </c>
       <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-    </row>
-    <row r="19" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L18" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M18" s="51"/>
+    </row>
+    <row r="19" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
         <v>348</v>
       </c>
@@ -8061,11 +8136,14 @@
         <v>244</v>
       </c>
       <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
+      <c r="L19" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="M19" s="51"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Maysoon Test cases were reviewed
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/TAWA_TestCases.xlsx
+++ b/Testing/Test Cases/TAWA_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ReservedTrips" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="660">
   <si>
     <t>ID</t>
   </si>
@@ -2561,6 +2561,30 @@
   </si>
   <si>
     <t>Maysoon Magdy</t>
+  </si>
+  <si>
+    <t>Missing SRS and actual result</t>
+  </si>
+  <si>
+    <t>Missing SRS, status and actual result</t>
+  </si>
+  <si>
+    <t>Missing bug ID</t>
+  </si>
+  <si>
+    <t>Many fields are missed</t>
+  </si>
+  <si>
+    <t>Missig bug id</t>
+  </si>
+  <si>
+    <t>Missing SRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahmoud Yasser </t>
+  </si>
+  <si>
+    <t>Missing bug id</t>
   </si>
 </sst>
 </file>
@@ -2691,7 +2715,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2742,6 +2766,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2750,7 +2794,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2828,7 +2872,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2922,6 +2965,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3297,244 +3346,244 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>611</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>612</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="57" t="s">
         <v>614</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>615</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="56" t="s">
         <v>616</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L2" s="57"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>617</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>618</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="57" t="s">
         <v>619</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="57" t="s">
         <v>620</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="56" t="s">
         <v>621</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="56" t="s">
         <v>622</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="56"/>
     </row>
     <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="56" t="s">
         <v>623</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="57" t="s">
         <v>624</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="57" t="s">
         <v>620</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="57" t="s">
         <v>625</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="56" t="s">
         <v>626</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="J4" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="57" t="s">
+      <c r="K4" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L4" s="57" t="s">
+      <c r="L4" s="56" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>628</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>629</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="57" t="s">
         <v>620</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="57" t="s">
         <v>630</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57" t="s">
+      <c r="H5" s="56"/>
+      <c r="I5" s="56" t="s">
         <v>631</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L5" s="57"/>
+      <c r="L5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="56" t="s">
         <v>632</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="56" t="s">
         <v>633</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="57" t="s">
         <v>634</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="57" t="s">
         <v>635</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58" t="s">
+      <c r="H6" s="56"/>
+      <c r="I6" s="57" t="s">
         <v>636</v>
       </c>
-      <c r="J6" s="57" t="s">
+      <c r="J6" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K6" s="57" t="s">
+      <c r="K6" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L6" s="57"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="56" t="s">
         <v>637</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>638</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="57" t="s">
         <v>634</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="57" t="s">
         <v>639</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58" t="s">
+      <c r="H7" s="56"/>
+      <c r="I7" s="57" t="s">
         <v>640</v>
       </c>
-      <c r="J7" s="57" t="s">
+      <c r="J7" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="57" t="s">
+      <c r="K7" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L7" s="57"/>
+      <c r="L7" s="56"/>
     </row>
     <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>641</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="56" t="s">
         <v>642</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="57" t="s">
         <v>643</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="56" t="s">
         <v>644</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57" t="s">
+      <c r="H8" s="56"/>
+      <c r="I8" s="56" t="s">
         <v>645</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="57" t="s">
+      <c r="K8" s="56" t="s">
         <v>651</v>
       </c>
-      <c r="L8" s="57"/>
+      <c r="L8" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3551,17 +3600,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" style="41" customWidth="1"/>
-    <col min="3" max="4" width="22" style="41" customWidth="1"/>
-    <col min="5" max="5" width="51.109375" style="41" customWidth="1"/>
-    <col min="6" max="6" width="50.109375" style="41" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="33.44140625" style="41" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" style="41" customWidth="1"/>
-    <col min="10" max="10" width="28" style="41" customWidth="1"/>
-    <col min="11" max="11" width="31.109375" style="41" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="41"/>
+    <col min="1" max="1" width="29.33203125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" style="40" customWidth="1"/>
+    <col min="3" max="4" width="22" style="40" customWidth="1"/>
+    <col min="5" max="5" width="51.109375" style="40" customWidth="1"/>
+    <col min="6" max="6" width="50.109375" style="40" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="33.44140625" style="40" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" style="40" customWidth="1"/>
+    <col min="10" max="10" width="28" style="40" customWidth="1"/>
+    <col min="11" max="11" width="31.109375" style="40" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3599,55 +3648,55 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="43" t="s">
         <v>515</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="47" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:11" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H3" s="11" t="s">
@@ -3656,7 +3705,7 @@
       <c r="I3" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="46" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3667,17 +3716,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="70.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" customWidth="1"/>
@@ -3689,9 +3738,10 @@
     <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="33" customFormat="1" ht="63" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>351</v>
       </c>
@@ -3734,8 +3784,11 @@
       <c r="N1" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="O1" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
         <v>352</v>
@@ -3765,9 +3818,14 @@
       <c r="M2" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N2" s="18"/>
-    </row>
-    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N2" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O2" s="63" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="18" t="s">
         <v>359</v>
@@ -3793,9 +3851,14 @@
       <c r="M3" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N3" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O3" s="63" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>364</v>
       </c>
@@ -3818,9 +3881,7 @@
       <c r="H4" s="21" t="s">
         <v>369</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>370</v>
-      </c>
+      <c r="I4" s="19"/>
       <c r="J4" s="19" t="s">
         <v>371</v>
       </c>
@@ -3831,9 +3892,14 @@
       <c r="M4" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="N4" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O4" s="63" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>373</v>
       </c>
@@ -3865,9 +3931,11 @@
       <c r="M5" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="N5" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>373</v>
       </c>
@@ -3897,9 +3965,14 @@
       <c r="M6" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N6" s="31"/>
-    </row>
-    <row r="7" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N6" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O6" s="64" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>382</v>
       </c>
@@ -3935,9 +4008,14 @@
       <c r="M7" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N7" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O7" s="64" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>388</v>
       </c>
@@ -3971,9 +4049,14 @@
       <c r="M8" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N8" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O8" s="64" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>394</v>
       </c>
@@ -4007,9 +4090,11 @@
       <c r="M9" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N9" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>400</v>
       </c>
@@ -4022,7 +4107,7 @@
       <c r="D10" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="31" t="s">
         <v>403</v>
       </c>
       <c r="F10" s="20" t="s">
@@ -4045,9 +4130,11 @@
       <c r="M10" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N10" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>407</v>
       </c>
@@ -4081,9 +4168,11 @@
       <c r="M11" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N11" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>413</v>
       </c>
@@ -4096,7 +4185,7 @@
       <c r="D12" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>416</v>
       </c>
       <c r="F12" s="20" t="s">
@@ -4119,9 +4208,11 @@
       <c r="M12" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="18" t="s">
         <v>420</v>
@@ -4153,10 +4244,15 @@
       <c r="M13" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="1:14" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="N13" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="O13" s="63" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="32" t="s">
         <v>425</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -4189,7 +4285,9 @@
       <c r="M14" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="N14" s="5"/>
+      <c r="N14" s="18" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4198,10 +4296,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4218,11 +4316,12 @@
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
     <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="34" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35"/>
+    <row r="1" spans="1:15" s="33" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4262,59 +4361,64 @@
       <c r="N1" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="O1" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>429</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>430</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="20" t="s">
         <v>431</v>
       </c>
       <c r="G2" s="14"/>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>432</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>433</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+      <c r="N2" s="33" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>435</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>436</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>430</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>438</v>
       </c>
       <c r="J3" t="s">
@@ -4326,21 +4430,27 @@
       <c r="M3" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
+      <c r="N3" s="33" t="s">
+        <v>658</v>
+      </c>
+      <c r="O3" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
         <v>440</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>441</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>442</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="33" t="s">
         <v>443</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="33" t="s">
         <v>444</v>
       </c>
       <c r="F4" s="20" t="s">
@@ -4349,7 +4459,7 @@
       <c r="G4" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="34" t="s">
         <v>432</v>
       </c>
       <c r="J4" t="s">
@@ -4361,21 +4471,27 @@
       <c r="M4" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+      <c r="N4" s="33" t="s">
+        <v>658</v>
+      </c>
+      <c r="O4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
         <v>447</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>448</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>449</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>443</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="33" t="s">
         <v>444</v>
       </c>
       <c r="F5" s="20" t="s">
@@ -4384,7 +4500,7 @@
       <c r="G5" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="35" t="s">
         <v>451</v>
       </c>
       <c r="J5" t="s">
@@ -4396,21 +4512,24 @@
       <c r="M5" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="N5" s="33" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
         <v>453</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>454</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>455</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>443</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="33" t="s">
         <v>444</v>
       </c>
       <c r="F6" s="20" t="s">
@@ -4419,7 +4538,7 @@
       <c r="G6" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="35" t="s">
         <v>457</v>
       </c>
       <c r="J6" t="s">
@@ -4431,21 +4550,24 @@
       <c r="M6" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
+      <c r="N6" s="33" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="s">
         <v>459</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>460</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>461</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="33" t="s">
         <v>443</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>444</v>
       </c>
       <c r="F7" s="20" t="s">
@@ -4454,7 +4576,7 @@
       <c r="G7" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="35" t="s">
         <v>463</v>
       </c>
       <c r="J7" t="s">
@@ -4466,38 +4588,46 @@
       <c r="M7" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39" t="s">
+      <c r="N7" s="33" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38" t="s">
         <v>464</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>465</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>466</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="30" t="s">
         <v>467</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="40" t="s">
+      <c r="G8" s="37"/>
+      <c r="H8" s="39" t="s">
         <v>468</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38" t="s">
+      <c r="I8" s="37"/>
+      <c r="J8" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38" t="s">
+      <c r="K8" s="37"/>
+      <c r="L8" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="37" t="s">
         <v>358</v>
       </c>
-      <c r="N8" s="38"/>
+      <c r="N8" s="33" t="s">
+        <v>658</v>
+      </c>
+      <c r="O8" t="s">
+        <v>659</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4511,7 +4641,7 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -4566,136 +4696,136 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>588</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>589</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="57" t="s">
         <v>590</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="57" t="s">
         <v>591</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>592</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="56" t="s">
         <v>594</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>595</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>596</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="59" t="s">
         <v>590</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="59" t="s">
         <v>597</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="59" t="s">
         <v>598</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="58" t="s">
         <v>599</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="54" t="s">
         <v>575</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="58" t="s">
         <v>600</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="58" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="56" t="s">
         <v>601</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="56" t="s">
         <v>602</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="57" t="s">
         <v>590</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="57" t="s">
         <v>603</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="57" t="s">
         <v>604</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="56" t="s">
         <v>605</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="J4" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="57" t="s">
+      <c r="K4" s="56" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>606</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>607</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="57" t="s">
         <v>590</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="57" t="s">
         <v>608</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="57" t="s">
         <v>609</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57" t="s">
+      <c r="H5" s="56"/>
+      <c r="I5" s="56" t="s">
         <v>610</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="56" t="s">
         <v>651</v>
       </c>
     </row>
@@ -4715,18 +4845,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" style="41" customWidth="1"/>
-    <col min="2" max="2" width="51.109375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="26" style="32" customWidth="1"/>
-    <col min="4" max="4" width="26" style="41" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" style="41" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" style="41" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="24" style="41" customWidth="1"/>
-    <col min="9" max="9" width="31.88671875" style="41" customWidth="1"/>
-    <col min="10" max="10" width="23" style="41" customWidth="1"/>
-    <col min="11" max="11" width="19" style="41" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="41"/>
+    <col min="1" max="1" width="24.88671875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="26" style="31" customWidth="1"/>
+    <col min="4" max="4" width="26" style="40" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="50.5546875" style="40" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="24" style="40" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" style="40" customWidth="1"/>
+    <col min="10" max="10" width="23" style="40" customWidth="1"/>
+    <col min="11" max="11" width="19" style="40" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4764,75 +4894,75 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:11" s="43" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="43" t="s">
         <v>520</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:11" s="43" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>521</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="43" t="s">
         <v>522</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:11" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="46" t="s">
         <v>508</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H4" s="11" t="s">
@@ -4841,80 +4971,80 @@
       <c r="I4" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="47" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+    <row r="7" spans="1:11" s="46" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -4923,27 +5053,27 @@
       <c r="I7" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
+    <row r="8" spans="1:11" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="47" t="s">
         <v>371</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -4952,53 +5082,53 @@
       <c r="I8" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="44" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:11" s="43" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="47" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:11" s="46" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -5007,53 +5137,53 @@
       <c r="I10" s="11" t="s">
         <v>525</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="44" t="s">
+    <row r="11" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="43" t="s">
         <v>526</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+    <row r="12" spans="1:11" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H12" s="11" t="s">
@@ -5062,134 +5192,134 @@
       <c r="I12" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+    <row r="13" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="43" t="s">
         <v>527</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I13" s="44" t="s">
+      <c r="I13" s="43" t="s">
         <v>528</v>
       </c>
-      <c r="J13" s="44" t="s">
+      <c r="J13" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:11" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="46" t="s">
         <v>530</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+    <row r="15" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="44" t="s">
+    <row r="16" spans="1:11" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I16" s="44" t="s">
+      <c r="I16" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+    <row r="17" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="G17" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H17" s="11" t="s">
@@ -5198,53 +5328,53 @@
       <c r="I17" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
+    <row r="19" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H19" s="11" t="s">
@@ -5253,27 +5383,27 @@
       <c r="I19" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H20" s="11" t="s">
@@ -5282,27 +5412,27 @@
       <c r="I20" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="F21" s="47" t="s">
+      <c r="F21" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H21" s="11" t="s">
@@ -5311,27 +5441,27 @@
       <c r="I21" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+    <row r="22" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H22" s="11" t="s">
@@ -5340,27 +5470,27 @@
       <c r="I22" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J22" s="47" t="s">
+      <c r="J22" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+    <row r="23" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="47" t="s">
+      <c r="F23" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="G23" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H23" s="11" t="s">
@@ -5369,161 +5499,161 @@
       <c r="I23" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="44" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
+    <row r="24" spans="1:10" s="43" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J24" s="44" t="s">
+      <c r="J24" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="44" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+    <row r="25" spans="1:10" s="43" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G25" s="49" t="s">
+      <c r="G25" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I25" s="44" t="s">
+      <c r="I25" s="43" t="s">
         <v>532</v>
       </c>
-      <c r="J25" s="44" t="s">
+      <c r="J25" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="44" t="s">
+    <row r="26" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I26" s="44" t="s">
+      <c r="I26" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="44" t="s">
+    <row r="27" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="F27" s="44" t="s">
+      <c r="F27" s="43" t="s">
         <v>509</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I27" s="44" t="s">
+      <c r="I27" s="43" t="s">
         <v>533</v>
       </c>
-      <c r="J27" s="44" t="s">
+      <c r="J27" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="46"/>
-      <c r="G28" s="46"/>
-    </row>
-    <row r="29" spans="1:10" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
+    <row r="28" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="45"/>
+      <c r="G28" s="45"/>
+    </row>
+    <row r="29" spans="1:10" s="43" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F29" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="49" t="s">
+      <c r="G29" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I29" s="44" t="s">
+      <c r="I29" s="43" t="s">
         <v>522</v>
       </c>
-      <c r="J29" s="44" t="s">
+      <c r="J29" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="47" t="s">
+    <row r="30" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="F30" s="47" t="s">
+      <c r="F30" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H30" s="11" t="s">
@@ -5532,80 +5662,80 @@
       <c r="I30" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J30" s="47" t="s">
+      <c r="J30" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
+    <row r="31" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="44" t="s">
+      <c r="E31" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="F31" s="44" t="s">
+      <c r="F31" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50" t="s">
+      <c r="H31" s="49"/>
+      <c r="I31" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J31" s="44" t="s">
+      <c r="J31" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="44" t="s">
+    <row r="32" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="F32" s="44" t="s">
+      <c r="F32" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="G32" s="49" t="s">
+      <c r="G32" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I32" s="50" t="s">
+      <c r="I32" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J32" s="44" t="s">
+      <c r="J32" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="47" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+    <row r="33" spans="1:10" s="46" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="F33" s="47" t="s">
+      <c r="F33" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="G33" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -5614,27 +5744,27 @@
       <c r="I33" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="J33" s="47" t="s">
+      <c r="J33" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="47" t="s">
+    <row r="34" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="46" t="s">
         <v>175</v>
       </c>
-      <c r="F34" s="47" t="s">
+      <c r="F34" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G34" s="48" t="s">
+      <c r="G34" s="47" t="s">
         <v>371</v>
       </c>
       <c r="H34" s="11" t="s">
@@ -5643,53 +5773,53 @@
       <c r="I34" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="44" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:10" s="43" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="G35" s="49" t="s">
+      <c r="G35" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I35" s="50" t="s">
+      <c r="I35" s="49" t="s">
         <v>523</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="J35" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="47" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
+    <row r="36" spans="1:10" s="46" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="F36" s="47" t="s">
+      <c r="F36" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="48" t="s">
+      <c r="G36" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H36" s="11" t="s">
@@ -5698,53 +5828,53 @@
       <c r="I36" s="11" t="s">
         <v>525</v>
       </c>
-      <c r="J36" s="47" t="s">
+      <c r="J36" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="44" t="s">
+    <row r="37" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="F37" s="44" t="s">
+      <c r="F37" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="49" t="s">
+      <c r="G37" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="43" t="s">
         <v>526</v>
       </c>
-      <c r="J37" s="44" t="s">
+      <c r="J37" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+    <row r="38" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="F38" s="47" t="s">
+      <c r="F38" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G38" s="48" t="s">
+      <c r="G38" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H38" s="11" t="s">
@@ -5753,134 +5883,134 @@
       <c r="I38" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J38" s="47" t="s">
+      <c r="J38" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="44" t="s">
+    <row r="39" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="44" t="s">
+      <c r="E39" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="F39" s="44" t="s">
+      <c r="F39" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G39" s="49" t="s">
+      <c r="G39" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I39" s="44" t="s">
+      <c r="I39" s="43" t="s">
         <v>528</v>
       </c>
-      <c r="J39" s="44" t="s">
+      <c r="J39" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+    <row r="40" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="47" t="s">
+      <c r="F40" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G40" s="48" t="s">
+      <c r="G40" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="I40" s="47" t="s">
+      <c r="I40" s="46" t="s">
         <v>530</v>
       </c>
-      <c r="J40" s="47" t="s">
+      <c r="J40" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="44" t="s">
+    <row r="41" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="44" t="s">
+      <c r="E41" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="F41" s="44" t="s">
+      <c r="F41" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="G41" s="49" t="s">
+      <c r="G41" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I41" s="44" t="s">
+      <c r="I41" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J41" s="44" t="s">
+      <c r="J41" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="44" t="s">
+    <row r="42" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="44" t="s">
+      <c r="E42" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="44" t="s">
+      <c r="F42" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="G42" s="49" t="s">
+      <c r="G42" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I42" s="44" t="s">
+      <c r="I42" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J42" s="44" t="s">
+      <c r="J42" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="47" t="s">
+    <row r="43" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="C43" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="F43" s="47" t="s">
+      <c r="F43" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G43" s="48" t="s">
+      <c r="G43" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H43" s="11" t="s">
@@ -5889,53 +6019,53 @@
       <c r="I43" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J43" s="47" t="s">
+      <c r="J43" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+    <row r="44" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="48" t="s">
+      <c r="C44" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="47" t="s">
+      <c r="E44" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="F44" s="47" t="s">
+      <c r="F44" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H44" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="J44" s="47" t="s">
+      <c r="J44" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
+    <row r="45" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="48" t="s">
+      <c r="C45" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="E45" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="F45" s="47" t="s">
+      <c r="F45" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G45" s="48" t="s">
+      <c r="G45" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H45" s="11" t="s">
@@ -5944,27 +6074,27 @@
       <c r="I45" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J45" s="47" t="s">
+      <c r="J45" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="47" t="s">
+    <row r="46" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="47" t="s">
+      <c r="E46" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="F46" s="47" t="s">
+      <c r="F46" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="48" t="s">
+      <c r="G46" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H46" s="11" t="s">
@@ -5973,27 +6103,27 @@
       <c r="I46" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J46" s="47" t="s">
+      <c r="J46" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="47" t="s">
+    <row r="47" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C47" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E47" s="47" t="s">
+      <c r="E47" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="F47" s="47" t="s">
+      <c r="F47" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G47" s="48" t="s">
+      <c r="G47" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H47" s="11" t="s">
@@ -6002,27 +6132,27 @@
       <c r="I47" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J47" s="47" t="s">
+      <c r="J47" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+    <row r="48" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="47" t="s">
+      <c r="B48" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="48" t="s">
+      <c r="C48" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E48" s="47" t="s">
+      <c r="E48" s="46" t="s">
         <v>512</v>
       </c>
-      <c r="F48" s="47" t="s">
+      <c r="F48" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G48" s="48" t="s">
+      <c r="G48" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H48" s="11" t="s">
@@ -6031,27 +6161,27 @@
       <c r="I48" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J48" s="47" t="s">
+      <c r="J48" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="47" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="47" t="s">
+    <row r="49" spans="1:10" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C49" s="48" t="s">
+      <c r="C49" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="47" t="s">
+      <c r="E49" s="46" t="s">
         <v>511</v>
       </c>
-      <c r="F49" s="47" t="s">
+      <c r="F49" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G49" s="48" t="s">
+      <c r="G49" s="47" t="s">
         <v>510</v>
       </c>
       <c r="H49" s="11" t="s">
@@ -6060,160 +6190,160 @@
       <c r="I49" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="J49" s="47" t="s">
+      <c r="J49" s="46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="44" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="44" t="s">
+    <row r="50" spans="1:10" s="43" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="49" t="s">
+      <c r="C50" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="44" t="s">
+      <c r="E50" s="43" t="s">
         <v>513</v>
       </c>
-      <c r="F50" s="44" t="s">
+      <c r="F50" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="G50" s="49" t="s">
+      <c r="G50" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I50" s="44" t="s">
+      <c r="I50" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J50" s="44" t="s">
+      <c r="J50" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="44" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="44" t="s">
+    <row r="51" spans="1:10" s="43" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E51" s="44" t="s">
+      <c r="E51" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="F51" s="44" t="s">
+      <c r="F51" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G51" s="49" t="s">
+      <c r="G51" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I51" s="44" t="s">
+      <c r="I51" s="43" t="s">
         <v>532</v>
       </c>
-      <c r="J51" s="44" t="s">
+      <c r="J51" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="44" t="s">
+    <row r="52" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="44" t="s">
+      <c r="E52" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="F52" s="44" t="s">
+      <c r="F52" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="G52" s="49" t="s">
+      <c r="G52" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="I52" s="44" t="s">
+      <c r="I52" s="43" t="s">
         <v>531</v>
       </c>
-      <c r="J52" s="44" t="s">
+      <c r="J52" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="44" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="44" t="s">
+    <row r="53" spans="1:10" s="43" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="44" t="s">
+      <c r="E53" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F53" s="44" t="s">
+      <c r="F53" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G53" s="49" t="s">
+      <c r="G53" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="I53" s="44" t="s">
+      <c r="I53" s="43" t="s">
         <v>533</v>
       </c>
-      <c r="J53" s="44" t="s">
+      <c r="J53" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="46"/>
-    </row>
-    <row r="55" spans="1:10" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A55" s="44" t="s">
+    <row r="54" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="45"/>
+    </row>
+    <row r="55" spans="1:10" s="43" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A55" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="E55" s="44" t="s">
+      <c r="E55" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="F55" s="44" t="s">
+      <c r="F55" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G55" s="49" t="s">
+      <c r="G55" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="J55" s="44" t="s">
+      <c r="J55" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="44" t="s">
+    <row r="56" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="43" t="s">
         <v>474</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="43" t="s">
         <v>475</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="E56" s="44" t="s">
+      <c r="E56" s="43" t="s">
         <v>476</v>
       </c>
-      <c r="F56" s="44" t="s">
+      <c r="F56" s="43" t="s">
         <v>477</v>
       </c>
-      <c r="G56" s="49" t="s">
+      <c r="G56" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="J56" s="44" t="s">
+      <c r="J56" s="43" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6233,18 +6363,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="62.33203125" style="41" customWidth="1"/>
-    <col min="6" max="6" width="46.5546875" style="41" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" style="32" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" style="41" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="41" customWidth="1"/>
-    <col min="10" max="10" width="28" style="41" customWidth="1"/>
-    <col min="11" max="11" width="31.109375" style="41" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="41"/>
+    <col min="1" max="1" width="25.6640625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="46.5546875" style="40" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="31" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="40" customWidth="1"/>
+    <col min="10" max="10" width="28" style="40" customWidth="1"/>
+    <col min="11" max="11" width="31.109375" style="40" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6282,295 +6412,295 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:11" s="41" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>497</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>498</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+    <row r="4" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="41" t="s">
         <v>499</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="42" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:11" s="41" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>500</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="42" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:11" s="41" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="41" t="s">
         <v>501</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="41" t="s">
         <v>502</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="41" t="s">
         <v>503</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="41" t="s">
         <v>504</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+    <row r="9" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="41" t="s">
         <v>504</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="41" t="s">
         <v>504</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="42" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="11" spans="1:11" s="41" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="41" t="s">
         <v>504</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="42" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+    <row r="12" spans="1:11" s="41" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
         <v>470</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="41" t="s">
         <v>471</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="42" t="s">
         <v>472</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="41" t="s">
         <v>473</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="41" t="s">
         <v>505</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="41" t="s">
         <v>506</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="41" t="s">
         <v>50</v>
       </c>
     </row>
@@ -7505,649 +7635,649 @@
       <c r="L1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="55" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>545</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51" t="s">
+      <c r="H2" s="50"/>
+      <c r="I2" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="50" t="s">
         <v>547</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M2" s="51"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>343</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="51" t="s">
         <v>548</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>574</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M3" s="51"/>
+      <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:13" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>247</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="51" t="s">
         <v>549</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51" t="s">
+      <c r="H4" s="50"/>
+      <c r="I4" s="50" t="s">
         <v>574</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="K4" s="50"/>
+      <c r="L4" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M4" s="51"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="51" t="s">
         <v>550</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51" t="s">
+      <c r="H5" s="50"/>
+      <c r="I5" s="50" t="s">
         <v>574</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51" t="s">
+      <c r="K5" s="50"/>
+      <c r="L5" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M5" s="51"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="60" t="s">
         <v>253</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="61" t="s">
         <v>551</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="60" t="s">
         <v>646</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="62" t="s">
         <v>575</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="61" t="s">
         <v>647</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61" t="s">
+      <c r="K6" s="60"/>
+      <c r="L6" s="60" t="s">
         <v>650</v>
       </c>
-      <c r="M6" s="61"/>
+      <c r="M6" s="60"/>
     </row>
     <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>256</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="51" t="s">
         <v>552</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="50"/>
+      <c r="I7" s="50" t="s">
         <v>576</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51" t="s">
+      <c r="K7" s="50"/>
+      <c r="L7" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M7" s="51"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>257</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="51" t="s">
         <v>553</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="51" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51" t="s">
+      <c r="H8" s="50"/>
+      <c r="I8" s="50" t="s">
         <v>576</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="J8" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51" t="s">
+      <c r="K8" s="50"/>
+      <c r="L8" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M8" s="51"/>
+      <c r="M8" s="50"/>
     </row>
     <row r="9" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="51" t="s">
         <v>554</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51" t="s">
+      <c r="H9" s="50"/>
+      <c r="I9" s="50" t="s">
         <v>577</v>
       </c>
-      <c r="J9" s="51" t="s">
+      <c r="J9" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51" t="s">
+      <c r="K9" s="50"/>
+      <c r="L9" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M9" s="51"/>
+      <c r="M9" s="50"/>
     </row>
     <row r="10" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>265</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="51" t="s">
         <v>555</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51" t="s">
+      <c r="H10" s="50"/>
+      <c r="I10" s="50" t="s">
         <v>578</v>
       </c>
-      <c r="J10" s="51" t="s">
+      <c r="J10" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51" t="s">
+      <c r="K10" s="50"/>
+      <c r="L10" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M10" s="51"/>
+      <c r="M10" s="50"/>
     </row>
     <row r="11" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="51" t="s">
         <v>556</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="51" t="s">
         <v>579</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51" t="s">
+      <c r="H11" s="50"/>
+      <c r="I11" s="50" t="s">
         <v>579</v>
       </c>
-      <c r="J11" s="51" t="s">
+      <c r="J11" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51" t="s">
+      <c r="K11" s="50"/>
+      <c r="L11" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M11" s="51"/>
+      <c r="M11" s="50"/>
     </row>
     <row r="12" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="51" t="s">
         <v>557</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="51" t="s">
         <v>558</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51" t="s">
+      <c r="H12" s="50"/>
+      <c r="I12" s="50" t="s">
         <v>579</v>
       </c>
-      <c r="J12" s="51" t="s">
+      <c r="J12" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51" t="s">
+      <c r="K12" s="50"/>
+      <c r="L12" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M12" s="51"/>
+      <c r="M12" s="50"/>
     </row>
     <row r="13" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="60" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="61" t="s">
         <v>573</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="61" t="s">
         <v>580</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="61" t="s">
         <v>559</v>
       </c>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="60" t="s">
         <v>646</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="H13" s="62" t="s">
         <v>581</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="61" t="s">
         <v>648</v>
       </c>
-      <c r="J13" s="61" t="s">
+      <c r="J13" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61" t="s">
+      <c r="K13" s="60"/>
+      <c r="L13" s="60" t="s">
         <v>650</v>
       </c>
-      <c r="M13" s="61"/>
+      <c r="M13" s="60"/>
     </row>
     <row r="14" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="50" t="s">
         <v>274</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="51" t="s">
         <v>560</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="51" t="s">
         <v>272</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51" t="s">
+      <c r="H14" s="50"/>
+      <c r="I14" s="50" t="s">
         <v>582</v>
       </c>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="50" t="s">
         <v>273</v>
       </c>
-      <c r="L14" s="51" t="s">
+      <c r="L14" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M14" s="51"/>
+      <c r="M14" s="50"/>
     </row>
     <row r="15" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="50" t="s">
         <v>277</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="50" t="s">
         <v>275</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="51" t="s">
         <v>561</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="51" t="s">
         <v>276</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51" t="s">
+      <c r="H15" s="50"/>
+      <c r="I15" s="50" t="s">
         <v>583</v>
       </c>
-      <c r="J15" s="51" t="s">
+      <c r="J15" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51" t="s">
+      <c r="K15" s="50"/>
+      <c r="L15" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M15" s="51"/>
+      <c r="M15" s="50"/>
     </row>
     <row r="16" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="52" t="s">
         <v>280</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="52" t="s">
         <v>278</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="53" t="s">
         <v>562</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="53" t="s">
         <v>279</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="52" t="s">
         <v>371</v>
       </c>
-      <c r="H16" s="55" t="s">
+      <c r="H16" s="54" t="s">
         <v>584</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="I16" s="52" t="s">
         <v>585</v>
       </c>
-      <c r="J16" s="53" t="s">
+      <c r="J16" s="52" t="s">
         <v>244</v>
       </c>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53" t="s">
+      <c r="K16" s="52"/>
+      <c r="L16" s="52" t="s">
         <v>650</v>
       </c>
-      <c r="M16" s="53"/>
+      <c r="M16" s="52"/>
     </row>
     <row r="17" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="50" t="s">
         <v>282</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>563</v>
       </c>
-      <c r="F17" s="52" t="s">
+      <c r="F17" s="51" t="s">
         <v>564</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51" t="s">
+      <c r="H17" s="50"/>
+      <c r="I17" s="50" t="s">
         <v>586</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="J17" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51" t="s">
+      <c r="K17" s="50"/>
+      <c r="L17" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M17" s="51"/>
+      <c r="M17" s="50"/>
     </row>
     <row r="18" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="50" t="s">
         <v>346</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="51" t="s">
         <v>347</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="51" t="s">
         <v>565</v>
       </c>
-      <c r="F18" s="52" t="s">
+      <c r="F18" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51" t="s">
+      <c r="H18" s="50"/>
+      <c r="I18" s="50" t="s">
         <v>587</v>
       </c>
-      <c r="J18" s="51" t="s">
+      <c r="J18" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51" t="s">
+      <c r="K18" s="50"/>
+      <c r="L18" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M18" s="51"/>
+      <c r="M18" s="50"/>
     </row>
     <row r="19" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="50" t="s">
         <v>348</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="50" t="s">
         <v>349</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="51" t="s">
         <v>566</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="51" t="s">
         <v>350</v>
       </c>
-      <c r="G19" s="51" t="s">
+      <c r="G19" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51" t="s">
+      <c r="H19" s="50"/>
+      <c r="I19" s="50" t="s">
         <v>574</v>
       </c>
-      <c r="J19" s="51" t="s">
+      <c r="J19" s="50" t="s">
         <v>244</v>
       </c>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51" t="s">
+      <c r="K19" s="50"/>
+      <c r="L19" s="50" t="s">
         <v>650</v>
       </c>
-      <c r="M19" s="51"/>
+      <c r="M19" s="50"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>